<commit_message>
Adding Simple Data Fetch from Excel
</commit_message>
<xml_diff>
--- a/DD_input.xlsx
+++ b/DD_input.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t xml:space="preserve">data</t>
   </si>
@@ -82,6 +82,33 @@
   </si>
   <si>
     <t xml:space="preserve">Delete_profile_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Message</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kdhfdjks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">regression34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mvncxmn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">regression24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kjgfkgjjkhkj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">regression25</t>
   </si>
 </sst>
 </file>
@@ -96,6 +123,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -183,8 +211,8 @@
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="79" zoomScaleNormal="79" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="79" zoomScaleNormal="79" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -281,9 +309,9 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="79" zoomScaleNormal="79" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="79" zoomScaleNormal="79" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -291,10 +319,55 @@
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -320,7 +393,7 @@
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>